<commit_message>
Add descriptive statistics to all registry data sets
</commit_message>
<xml_diff>
--- a/Data/Order_list/Variabler_GSI.xlsx
+++ b/Data/Order_list/Variabler_GSI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\Data\Order_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F62AAB-2EB4-4830-8593-6941F492E242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A263442D-94F6-4F4D-AA91-F9EC5D632426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skoleporten" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="201">
   <si>
     <t>Skoletype</t>
   </si>
@@ -235,9 +235,6 @@
     <t>Kompetansekrav for tilsetting, jf. opplæringsloven § 10-1 og friskoleloven § 4-2</t>
   </si>
   <si>
-    <t>Kompetansekrav fro undervisning i fag de underviser i, for lærere oppgitt i linje 35 og 36, jf. opplæringsloven § 10-2 og friskoleloven § 4-2</t>
-  </si>
-  <si>
     <t>D. Spesialundervisning</t>
   </si>
   <si>
@@ -340,9 +337,6 @@
     <t>Leirskole</t>
   </si>
   <si>
-    <t>SFO</t>
-  </si>
-  <si>
     <t>Foreldrebetaling</t>
   </si>
   <si>
@@ -374,13 +368,277 @@
   </si>
   <si>
     <t>Utfyllers e-post</t>
+  </si>
+  <si>
+    <t>School contribution Year 1--4</t>
+  </si>
+  <si>
+    <t>School contribution Year 5--7</t>
+  </si>
+  <si>
+    <t>School contribution Year 8--10</t>
+  </si>
+  <si>
+    <t>Number of students</t>
+  </si>
+  <si>
+    <t>Uncertainty</t>
+  </si>
+  <si>
+    <t>Teacher-assigned grades</t>
+  </si>
+  <si>
+    <t>Exam grades</t>
+  </si>
+  <si>
+    <t>Primary school grades</t>
+  </si>
+  <si>
+    <t>National test Year 5</t>
+  </si>
+  <si>
+    <t>Competency Level 1</t>
+  </si>
+  <si>
+    <t>Competency Level 2</t>
+  </si>
+  <si>
+    <t>Competency Level 3</t>
+  </si>
+  <si>
+    <t>Competency Level 4</t>
+  </si>
+  <si>
+    <t>Competency Level 5</t>
+  </si>
+  <si>
+    <t>Spread upper bound</t>
+  </si>
+  <si>
+    <t>Spread lower bound</t>
+  </si>
+  <si>
+    <t>National tests lower secondary school</t>
+  </si>
+  <si>
+    <t>National tests exempted or not participated</t>
+  </si>
+  <si>
+    <t>National test Year 5 2009--2013</t>
+  </si>
+  <si>
+    <t>National test lower secondary 2009--2013</t>
+  </si>
+  <si>
+    <t>Name of unit</t>
+  </si>
+  <si>
+    <t>Company organisation number</t>
+  </si>
+  <si>
+    <t>Firm organisation number</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Institution type</t>
+  </si>
+  <si>
+    <t>Operation responsibility</t>
+  </si>
+  <si>
+    <t>Post number / place</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Responder's email</t>
+  </si>
+  <si>
+    <t>What is this school's lowest year level?</t>
+  </si>
+  <si>
+    <t>What is this school's highest year level?</t>
+  </si>
+  <si>
+    <t>Number of pupils in this school</t>
+  </si>
+  <si>
+    <t>How many of the students mentioned in Line 15 are asylumn seekers?</t>
+  </si>
+  <si>
+    <t>Students who need sign language and Braill training</t>
+  </si>
+  <si>
+    <t>Home schooling--parents teaching their own children</t>
+  </si>
+  <si>
+    <t>Students who did not attend at the beginning of the school year</t>
+  </si>
+  <si>
+    <t>Total teaching hours per annual</t>
+  </si>
+  <si>
+    <t>Total number of hours carried out by teaching staff for literacy purposes</t>
+  </si>
+  <si>
+    <t>Total number of hours carried out by teaching staff</t>
+  </si>
+  <si>
+    <t>Total number of hours carried out by teaching assistants</t>
+  </si>
+  <si>
+    <t>Number of hours for administrative and pedagogic leadership tasks</t>
+  </si>
+  <si>
+    <t>Partial loading adjustment</t>
+  </si>
+  <si>
+    <t>Teaching-related labour-year (1 full labour-year = 100)</t>
+  </si>
+  <si>
+    <t>Non-teaching-related labour-year (1 full labour-year = 100)</t>
+  </si>
+  <si>
+    <t>Labour-year carried out by assistants</t>
+  </si>
+  <si>
+    <t>Labour-year carried out by other personnel</t>
+  </si>
+  <si>
+    <t>Number of teachers and assistants</t>
+  </si>
+  <si>
+    <t>Kompetansekrav for undervisning i fag de underviser i, for lærere oppgitt i linje 35 og 36, jf. opplæringsloven § 10-2 og friskoleloven § 4-2</t>
+  </si>
+  <si>
+    <t>Alternate arena of tuition</t>
+  </si>
+  <si>
+    <t>How many pupils that receive special needs education based on caretaker/guardian decisions</t>
+  </si>
+  <si>
+    <t>Pupils in designated areas for special needs education</t>
+  </si>
+  <si>
+    <t>Organisation of special needs education</t>
+  </si>
+  <si>
+    <t>Number of students receiving extra special need education carried out by teaching staff</t>
+  </si>
+  <si>
+    <t>Number of students who receive extra hours with teaching assistants as part of the caretaker decisions about special need education</t>
+  </si>
+  <si>
+    <t>Total numbers of caretaker/gardian decisions</t>
+  </si>
+  <si>
+    <t>Students with special education needs from other municipalities</t>
+  </si>
+  <si>
+    <t>Students receiving special language training by year levels</t>
+  </si>
+  <si>
+    <t>Students in delicated tuition groups</t>
+  </si>
+  <si>
+    <t>How many of the students mentioned in Line 15 are financed by other minicipality, set forth by s. 18-1 Education Act (only applicable to public schools)</t>
+  </si>
+  <si>
+    <t>Employment standard requirement under s. 10-1 of Education Act</t>
+  </si>
+  <si>
+    <t>For teachers mentioned in Line 35 and 36, the employment standard requirement for the subjects they teach, as per s. 10-2 of Education Act and s. 4-2 of Private School Act</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students receiving vocational/facilitated training in both Norwegian and their native languages, as per s. 2-8 of Education Act and s. 3-5 of Private School Act </t>
+  </si>
+  <si>
+    <t>Students with individualised Norwegian language training from other municipalities</t>
+  </si>
+  <si>
+    <t>Teaching language</t>
+  </si>
+  <si>
+    <t>Student groups</t>
+  </si>
+  <si>
+    <t>Sami or Finnish</t>
+  </si>
+  <si>
+    <t>Students with foreign language/language enforcement/labour life-related subjects</t>
+  </si>
+  <si>
+    <t>Students without foreign language/language enforcement/labour life-related subjects</t>
+  </si>
+  <si>
+    <t>Sum of the previous two</t>
+  </si>
+  <si>
+    <t>Students with elective subjects</t>
+  </si>
+  <si>
+    <t>Subjects from upper secondary schools instead of elective subjects</t>
+  </si>
+  <si>
+    <t>Number of students with and without electives</t>
+  </si>
+  <si>
+    <t>Annual physical activity hours for Year 5--7</t>
+  </si>
+  <si>
+    <t>Physical activity resources for Year 5--7</t>
+  </si>
+  <si>
+    <t>Number of students and total number of hours devoted for free homework help for Year 1--10</t>
+  </si>
+  <si>
+    <t>Means of transportation to school</t>
+  </si>
+  <si>
+    <t>Re-assignment of hourly number (25% rule)</t>
+  </si>
+  <si>
+    <t>Lower secondary students who take upper secondary subjects</t>
+  </si>
+  <si>
+    <t>Labour camp</t>
+  </si>
+  <si>
+    <t>After-school organised learning sessions</t>
+  </si>
+  <si>
+    <t>SFO (skolefritidsordning)</t>
+  </si>
+  <si>
+    <t>Parental payments</t>
+  </si>
+  <si>
+    <t>Subsidised payments</t>
+  </si>
+  <si>
+    <t>Organisation of PPT as per s. 5-6 of Education Act</t>
+  </si>
+  <si>
+    <t>Coordination with PPT in upper secondary schools</t>
+  </si>
+  <si>
+    <t>Streams and educational background into standardised PPT labour-years</t>
+  </si>
+  <si>
+    <t>Other municipalities that utilise this unit's PPT</t>
+  </si>
+  <si>
+    <t>Municipality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,8 +654,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,6 +693,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -429,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -439,19 +722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -460,11 +731,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,62 +1032,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>27</v>
+      <c r="C3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -809,16 +1100,19 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -826,33 +1120,39 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>27</v>
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>27</v>
+      <c r="C6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -860,16 +1160,19 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -877,33 +1180,39 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>27</v>
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>27</v>
+      <c r="C9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -911,16 +1220,19 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -928,33 +1240,39 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
+      <c r="C12" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -962,16 +1280,19 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -979,33 +1300,39 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
+        <v>117</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>27</v>
+      <c r="C15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1013,16 +1340,19 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1030,33 +1360,39 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>27</v>
+        <v>117</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>27</v>
+      <c r="C18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1064,33 +1400,39 @@
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>27</v>
+      <c r="C20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1098,16 +1440,19 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>27</v>
+        <v>122</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1115,16 +1460,19 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>27</v>
+        <v>123</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1132,16 +1480,19 @@
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>27</v>
+        <v>124</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1149,16 +1500,19 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1166,16 +1520,19 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>27</v>
+        <v>127</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1183,16 +1540,19 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>27</v>
+        <v>128</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1200,135 +1560,159 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>27</v>
+        <v>117</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>27</v>
+      <c r="C28" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>27</v>
+      <c r="C29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>27</v>
+      <c r="C30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>27</v>
+      <c r="C31" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>27</v>
+      <c r="C32" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>27</v>
+      <c r="C33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
       <c r="B34" t="s">
         <v>24</v>
       </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>27</v>
+      <c r="C34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1336,16 +1720,19 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>27</v>
+        <v>127</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1353,224 +1740,264 @@
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>27</v>
+        <v>128</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
       <c r="B37" t="s">
         <v>23</v>
       </c>
-      <c r="C37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>27</v>
+      <c r="C37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>27</v>
+      <c r="C38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>27</v>
+      <c r="C39" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>15</v>
       </c>
-      <c r="C40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>27</v>
+      <c r="C40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
       </c>
-      <c r="C41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>27</v>
+      <c r="C41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
       <c r="B42" t="s">
         <v>17</v>
       </c>
-      <c r="C42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>27</v>
+      <c r="C42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>27</v>
+      <c r="C43" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>27</v>
+      <c r="C44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>27</v>
+      <c r="C45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>27</v>
+      <c r="C46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>27</v>
+      <c r="C47" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>27</v>
+      <c r="C48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
       </c>
       <c r="E48" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:B32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1579,779 +2006,990 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B120800-2565-4143-88BA-0E02A2DB0EAD}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="21.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="C3" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="C6" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="C7" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="C8" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="C9" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="C12" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="C13" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="C14" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="9"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="12"/>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="B38" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="11" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="11" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="11" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C41" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="11" t="s">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C42" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="11" t="s">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C43" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="11" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C44" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="11" t="s">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C45" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="11" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="B47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-    </row>
-    <row r="47" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B47" s="11" t="s">
+    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C48" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" s="11" t="s">
+    <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C49" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="11" t="s">
+    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C50" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B50" s="11" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+    </row>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="B52" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B52" s="11" t="s">
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C53" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B53" s="11" t="s">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C54" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B54" s="11" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+    </row>
+    <row r="56" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-    </row>
-    <row r="56" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="B56" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="C56" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C57" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B57" s="11" t="s">
+    <row r="58" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C58" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="11" t="s">
+    <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C59" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B59" s="11" t="s">
+    <row r="60" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C60" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" s="11" t="s">
+    <row r="61" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C61" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B61" s="11" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+    </row>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="B63" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-    </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="C64" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C65" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="10" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D67" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B65" s="11" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="B68" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="10" t="s">
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="10" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C69" s="10" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D71" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B70" s="11" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C72" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D72" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B71" s="11" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C73" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D73" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B72" s="11" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="12"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+    </row>
+    <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="B75" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D75" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C73" s="10" t="s">
+    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D76" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-    </row>
-    <row r="75" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B75" s="11" t="s">
+    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C77" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D77" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B76" s="11" t="s">
+    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C76" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B77" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C78" s="10" t="s">
+      <c r="C78" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D78" s="6" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2571,18 +3209,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2605,18 +3243,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959D5EEA-D387-4C47-85A7-E3C536B69AB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68834D28-CEB4-441B-9571-DBCDCF5E465B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959D5EEA-D387-4C47-85A7-E3C536B69AB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>